<commit_message>
Genes of interest, network metrics
Update of 'Supplementary Tables
</commit_message>
<xml_diff>
--- a/paper/supplementary_tables.xlsx
+++ b/paper/supplementary_tables.xlsx
@@ -11,6 +11,8 @@
     <sheet name="Supplementary Table S1" sheetId="2" r:id="rId2"/>
     <sheet name="Supplementary Table S2" sheetId="3" r:id="rId3"/>
     <sheet name="Supplementary Table S3" sheetId="4" r:id="rId4"/>
+    <sheet name="Supplementary Table S4" sheetId="5" r:id="rId5"/>
+    <sheet name="Supplementary Table S5" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -354,7 +356,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -405,6 +407,30 @@
       <c r="B4" t="inlineStr">
         <is>
           <t>Characteristic of the training and test subsets of the GSE16560 cohort. For modeling of overall survival, the GSE16560 cohort was randomly split into a training and a test subset in a  2:1 ratio. Numeric characteristics of the subsets are presented as medians with interquartile ranges (IQR) and ranges. Qualitative variables are presented as percentages of categories within the complete observation set.</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Supplementary Table S4</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Collagen-related genes and their classification.</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Supplementary Table S5</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Vertex importance statistics for co-expression networks of the collagen-related transcripts. The co-expression networks were built for in the pooled GEO, TCGA, and DKFZ cohorts for transcripts with pairwise correlation of expression levels with Spearman's rho &gt;= 0.5. Metrics of importance of the vertices of the co-expression networks, degree, hub score, betweenness, and transitivity, were computed. Top five vertices with the largest hub score per cohort are presented. The full table is available as a supplementary Excel file.</t>
         </is>
       </c>
     </row>
@@ -1479,4 +1505,4511 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C56"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" s="1" customFormat="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Functional classification</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Gene symbol</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Entrez ID</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>proline metabolism</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>ALDH18A1</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>5832</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>proline metabolism</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>PEPD</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>5184</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>proline metabolism</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>PYCR1</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>5831</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>collagen modification</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>LOX</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>4015</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>collagen modification</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>LOXL1</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>4016</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>collagen modification</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>LOXL2</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>4017</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>collagen modification</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>P4HA1</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>5033</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>collagen modification</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>P4HA2</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>8974</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>collagen modification</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>P4HB</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>5034</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>collagen modification</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>PLOD1</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>5351</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>collagen modification</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>PLOD2</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>5352</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>collagen modification</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>PLOD3</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>8985</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>collagen modification</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>PPIB</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>5479</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>ECM component</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>COL11A1</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>1301</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>ECM component</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>COL11A2</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>1302</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>ECM component</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>COL14A1</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>7373</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>ECM component</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>COL15A1</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>1306</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>ECM component</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>COL16A1</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>1307</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>ECM component</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>COL17A1</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>1308</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>ECM component</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>COL18A1</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>80781</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>ECM component</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>COL19A1</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>1310</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>ECM component</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>COL1A1</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>1277</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>ECM component</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>COL1A2</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>1278</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>ECM component</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>COL2A1</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>1280</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>ECM component</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>COL3A1</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>1281</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>ECM component</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>COL4A1</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>1282</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>ECM component</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>COL4A2</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>1284</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>ECM component</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>COL4A3</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>1285</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>ECM component</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>COL4A5</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>1287</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>ECM component</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>COL4A6</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>1288</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>ECM component</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>COL5A1</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>1289</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>ECM component</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>COL5A2</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>1290</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>ECM component</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>COL6A1</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>1291</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>ECM component</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>COL6A2</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>1292</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>ECM component</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>COL6A3</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>1293</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>ECM component</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>COL7A1</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>1294</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>ECM component</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>COL9A1</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>1297</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>ECM component</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>COL9A2</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>1298</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>ECM component</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>COL9A3</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>1299</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>ECM component</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>LAMA3</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>3909</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>ECM component</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>LAMB3</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>3914</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>ECM component</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>LAMC2</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>3918</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>ECM processing</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>ADAMTS2</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>9509</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>ECM processing</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>BMP1</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>649</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>ECM processing</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>CTSS</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>1520</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>ECM processing</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>MMP13</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>4322</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>ECM processing</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>MMP7</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>4316</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>ECM processing</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>MMP9</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>4318</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>ECM processing</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>PCOLCE</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>5118</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>ECM processing</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>PCOLCE2</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>26577</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>ECM processing</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>SERPINH1</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>871</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>adhesion</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>CD151</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>977</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>adhesion</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>DST</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>667</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>adhesion</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>ITGA6</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>3655</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>adhesion</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>ITGB4</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>3691</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:G124"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" s="1" customFormat="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Cohort</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Gene symbol</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Functional classification</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Degree</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Hub score</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Betweenness</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Transitivity</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>pooled GEO</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>ADAMTS2</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>ECM processing</t>
+        </is>
+      </c>
+      <c r="D2">
+        <v>12</v>
+      </c>
+      <c r="E2">
+        <v>0.58</v>
+      </c>
+      <c r="F2">
+        <v>0.016</v>
+      </c>
+      <c r="G2">
+        <v>0.98</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>pooled GEO</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>ALDH18A1</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>proline metabolism</t>
+        </is>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>pooled GEO</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>BMP1</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>ECM processing</t>
+        </is>
+      </c>
+      <c r="D4">
+        <v>12</v>
+      </c>
+      <c r="E4">
+        <v>0.55</v>
+      </c>
+      <c r="F4">
+        <v>0.42</v>
+      </c>
+      <c r="G4">
+        <v>0.82</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>pooled GEO</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>COL14A1</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>ECM component</t>
+        </is>
+      </c>
+      <c r="D5">
+        <v>12</v>
+      </c>
+      <c r="E5">
+        <v>0.5</v>
+      </c>
+      <c r="F5">
+        <v>0.35</v>
+      </c>
+      <c r="G5">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>pooled GEO</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>COL15A1</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>ECM component</t>
+        </is>
+      </c>
+      <c r="D6">
+        <v>15</v>
+      </c>
+      <c r="E6">
+        <v>0.78</v>
+      </c>
+      <c r="F6">
+        <v>0.016</v>
+      </c>
+      <c r="G6">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>pooled GEO</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>COL16A1</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>ECM component</t>
+        </is>
+      </c>
+      <c r="D7">
+        <v>19</v>
+      </c>
+      <c r="E7">
+        <v>0.93</v>
+      </c>
+      <c r="F7">
+        <v>0.19</v>
+      </c>
+      <c r="G7">
+        <v>0.74</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>pooled GEO</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>COL17A1</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>ECM component</t>
+        </is>
+      </c>
+      <c r="D8">
+        <v>3</v>
+      </c>
+      <c r="E8">
+        <v>0.032</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>pooled GEO</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>COL18A1</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>ECM component</t>
+        </is>
+      </c>
+      <c r="D9">
+        <v>13</v>
+      </c>
+      <c r="E9">
+        <v>0.61</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>0.8100000000000001</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>pooled GEO</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>COL1A1</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>ECM component</t>
+        </is>
+      </c>
+      <c r="D10">
+        <v>16</v>
+      </c>
+      <c r="E10">
+        <v>0.87</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>0.87</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>pooled GEO</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>COL1A2</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>ECM component</t>
+        </is>
+      </c>
+      <c r="D11">
+        <v>16</v>
+      </c>
+      <c r="E11">
+        <v>0.87</v>
+      </c>
+      <c r="F11">
+        <v>0.065</v>
+      </c>
+      <c r="G11">
+        <v>0.87</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>pooled GEO</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>COL3A1</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>ECM component</t>
+        </is>
+      </c>
+      <c r="D12">
+        <v>13</v>
+      </c>
+      <c r="E12">
+        <v>0.75</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <v>0.97</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>pooled GEO</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>COL4A1</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>ECM component</t>
+        </is>
+      </c>
+      <c r="D13">
+        <v>17</v>
+      </c>
+      <c r="E13">
+        <v>0.91</v>
+      </c>
+      <c r="F13">
+        <v>0.016</v>
+      </c>
+      <c r="G13">
+        <v>0.83</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>pooled GEO</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>COL4A2</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>ECM component</t>
+        </is>
+      </c>
+      <c r="D14">
+        <v>19</v>
+      </c>
+      <c r="E14">
+        <v>0.98</v>
+      </c>
+      <c r="F14">
+        <v>0.097</v>
+      </c>
+      <c r="G14">
+        <v>0.74</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>pooled GEO</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>COL4A5</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>ECM component</t>
+        </is>
+      </c>
+      <c r="D15">
+        <v>2</v>
+      </c>
+      <c r="E15">
+        <v>0.046</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+      <c r="G15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>pooled GEO</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>COL4A6</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>ECM component</t>
+        </is>
+      </c>
+      <c r="D16">
+        <v>4</v>
+      </c>
+      <c r="E16">
+        <v>0.12</v>
+      </c>
+      <c r="F16">
+        <v>0.016</v>
+      </c>
+      <c r="G16">
+        <v>0.67</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>pooled GEO</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>COL5A1</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>ECM component</t>
+        </is>
+      </c>
+      <c r="D17">
+        <v>19</v>
+      </c>
+      <c r="E17">
+        <v>1</v>
+      </c>
+      <c r="F17">
+        <v>0.13</v>
+      </c>
+      <c r="G17">
+        <v>0.74</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>pooled GEO</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>COL5A2</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>ECM component</t>
+        </is>
+      </c>
+      <c r="D18">
+        <v>14</v>
+      </c>
+      <c r="E18">
+        <v>0.73</v>
+      </c>
+      <c r="F18">
+        <v>0.065</v>
+      </c>
+      <c r="G18">
+        <v>0.89</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>pooled GEO</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>COL6A1</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>ECM component</t>
+        </is>
+      </c>
+      <c r="D19">
+        <v>17</v>
+      </c>
+      <c r="E19">
+        <v>0.74</v>
+      </c>
+      <c r="F19">
+        <v>0.48</v>
+      </c>
+      <c r="G19">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>pooled GEO</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>COL6A2</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>ECM component</t>
+        </is>
+      </c>
+      <c r="D20">
+        <v>18</v>
+      </c>
+      <c r="E20">
+        <v>0.8</v>
+      </c>
+      <c r="F20">
+        <v>0.44</v>
+      </c>
+      <c r="G20">
+        <v>0.66</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>pooled GEO</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>COL6A3</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>ECM component</t>
+        </is>
+      </c>
+      <c r="D21">
+        <v>19</v>
+      </c>
+      <c r="E21">
+        <v>0.92</v>
+      </c>
+      <c r="F21">
+        <v>0.27</v>
+      </c>
+      <c r="G21">
+        <v>0.72</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>pooled GEO</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>COL7A1</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>ECM component</t>
+        </is>
+      </c>
+      <c r="D22">
+        <v>9</v>
+      </c>
+      <c r="E22">
+        <v>0.3</v>
+      </c>
+      <c r="F22">
+        <v>1</v>
+      </c>
+      <c r="G22">
+        <v>0.61</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>pooled GEO</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>CTSS</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>ECM processing</t>
+        </is>
+      </c>
+      <c r="D23">
+        <v>1</v>
+      </c>
+      <c r="E23">
+        <v>0</v>
+      </c>
+      <c r="F23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>pooled GEO</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>DST</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>adhesion</t>
+        </is>
+      </c>
+      <c r="D24">
+        <v>1</v>
+      </c>
+      <c r="E24">
+        <v>0.002</v>
+      </c>
+      <c r="F24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>pooled GEO</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>ITGB4</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>adhesion</t>
+        </is>
+      </c>
+      <c r="D25">
+        <v>8</v>
+      </c>
+      <c r="E25">
+        <v>0.23</v>
+      </c>
+      <c r="F25">
+        <v>0.081</v>
+      </c>
+      <c r="G25">
+        <v>0.61</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>pooled GEO</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>LAMB3</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>ECM component</t>
+        </is>
+      </c>
+      <c r="D26">
+        <v>4</v>
+      </c>
+      <c r="E26">
+        <v>0.038</v>
+      </c>
+      <c r="F26">
+        <v>0.4</v>
+      </c>
+      <c r="G26">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>pooled GEO</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>LOXL1</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>collagen modification</t>
+        </is>
+      </c>
+      <c r="D27">
+        <v>13</v>
+      </c>
+      <c r="E27">
+        <v>0.64</v>
+      </c>
+      <c r="F27">
+        <v>0</v>
+      </c>
+      <c r="G27">
+        <v>0.96</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>pooled GEO</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>MMP9</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>ECM processing</t>
+        </is>
+      </c>
+      <c r="D28">
+        <v>1</v>
+      </c>
+      <c r="E28">
+        <v>0</v>
+      </c>
+      <c r="F28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>pooled GEO</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>P4HB</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>collagen modification</t>
+        </is>
+      </c>
+      <c r="D29">
+        <v>3</v>
+      </c>
+      <c r="E29">
+        <v>0</v>
+      </c>
+      <c r="F29">
+        <v>0.048</v>
+      </c>
+      <c r="G29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>pooled GEO</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>PCOLCE</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>ECM processing</t>
+        </is>
+      </c>
+      <c r="D30">
+        <v>18</v>
+      </c>
+      <c r="E30">
+        <v>0.86</v>
+      </c>
+      <c r="F30">
+        <v>0.11</v>
+      </c>
+      <c r="G30">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>pooled GEO</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>PCOLCE2</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>ECM processing</t>
+        </is>
+      </c>
+      <c r="D31">
+        <v>2</v>
+      </c>
+      <c r="E31">
+        <v>0.077</v>
+      </c>
+      <c r="F31">
+        <v>0</v>
+      </c>
+      <c r="G31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>pooled GEO</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>PLOD1</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>collagen modification</t>
+        </is>
+      </c>
+      <c r="D32">
+        <v>1</v>
+      </c>
+      <c r="E32">
+        <v>0</v>
+      </c>
+      <c r="F32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>pooled GEO</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>PLOD3</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>collagen modification</t>
+        </is>
+      </c>
+      <c r="D33">
+        <v>1</v>
+      </c>
+      <c r="E33">
+        <v>0</v>
+      </c>
+      <c r="F33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>pooled GEO</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>PPIB</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>collagen modification</t>
+        </is>
+      </c>
+      <c r="D34">
+        <v>1</v>
+      </c>
+      <c r="E34">
+        <v>0</v>
+      </c>
+      <c r="F34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>pooled GEO</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>PYCR1</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>proline metabolism</t>
+        </is>
+      </c>
+      <c r="D35">
+        <v>1</v>
+      </c>
+      <c r="E35">
+        <v>0</v>
+      </c>
+      <c r="F35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>pooled GEO</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>SERPINH1</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>ECM processing</t>
+        </is>
+      </c>
+      <c r="D36">
+        <v>15</v>
+      </c>
+      <c r="E36">
+        <v>0.72</v>
+      </c>
+      <c r="F36">
+        <v>0.11</v>
+      </c>
+      <c r="G36">
+        <v>0.87</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>TCGA</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>ADAMTS2</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>ECM processing</t>
+        </is>
+      </c>
+      <c r="D37">
+        <v>21</v>
+      </c>
+      <c r="E37">
+        <v>0.87</v>
+      </c>
+      <c r="F37">
+        <v>0.51</v>
+      </c>
+      <c r="G37">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>TCGA</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>BMP1</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>ECM processing</t>
+        </is>
+      </c>
+      <c r="D38">
+        <v>16</v>
+      </c>
+      <c r="E38">
+        <v>0.59</v>
+      </c>
+      <c r="F38">
+        <v>0.32</v>
+      </c>
+      <c r="G38">
+        <v>0.79</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>TCGA</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>CD151</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>adhesion</t>
+        </is>
+      </c>
+      <c r="D39">
+        <v>1</v>
+      </c>
+      <c r="E39">
+        <v>6.8e-18</v>
+      </c>
+      <c r="F39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>TCGA</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>COL11A1</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>ECM component</t>
+        </is>
+      </c>
+      <c r="D40">
+        <v>5</v>
+      </c>
+      <c r="E40">
+        <v>0.18</v>
+      </c>
+      <c r="F40">
+        <v>0</v>
+      </c>
+      <c r="G40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>TCGA</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>COL11A2</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>ECM component</t>
+        </is>
+      </c>
+      <c r="D41">
+        <v>1</v>
+      </c>
+      <c r="E41">
+        <v>0.0042</v>
+      </c>
+      <c r="F41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>TCGA</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>COL14A1</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>ECM component</t>
+        </is>
+      </c>
+      <c r="D42">
+        <v>21</v>
+      </c>
+      <c r="E42">
+        <v>0.8</v>
+      </c>
+      <c r="F42">
+        <v>0.74</v>
+      </c>
+      <c r="G42">
+        <v>0.71</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>TCGA</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>COL15A1</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>ECM component</t>
+        </is>
+      </c>
+      <c r="D43">
+        <v>22</v>
+      </c>
+      <c r="E43">
+        <v>0.93</v>
+      </c>
+      <c r="F43">
+        <v>0.073</v>
+      </c>
+      <c r="G43">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>TCGA</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>COL16A1</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>ECM component</t>
+        </is>
+      </c>
+      <c r="D44">
+        <v>24</v>
+      </c>
+      <c r="E44">
+        <v>0.9399999999999999</v>
+      </c>
+      <c r="F44">
+        <v>0.59</v>
+      </c>
+      <c r="G44">
+        <v>0.6899999999999999</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>TCGA</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>COL17A1</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>ECM component</t>
+        </is>
+      </c>
+      <c r="D45">
+        <v>7</v>
+      </c>
+      <c r="E45">
+        <v>0.025</v>
+      </c>
+      <c r="F45">
+        <v>0.18</v>
+      </c>
+      <c r="G45">
+        <v>0.57</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>TCGA</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>COL18A1</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>ECM component</t>
+        </is>
+      </c>
+      <c r="D46">
+        <v>19</v>
+      </c>
+      <c r="E46">
+        <v>0.71</v>
+      </c>
+      <c r="F46">
+        <v>1</v>
+      </c>
+      <c r="G46">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>TCGA</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>COL19A1</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>ECM component</t>
+        </is>
+      </c>
+      <c r="D47">
+        <v>2</v>
+      </c>
+      <c r="E47">
+        <v>0.052</v>
+      </c>
+      <c r="F47">
+        <v>0</v>
+      </c>
+      <c r="G47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>TCGA</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>COL1A1</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>ECM component</t>
+        </is>
+      </c>
+      <c r="D48">
+        <v>19</v>
+      </c>
+      <c r="E48">
+        <v>0.87</v>
+      </c>
+      <c r="F48">
+        <v>0.012</v>
+      </c>
+      <c r="G48">
+        <v>0.88</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>TCGA</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>COL1A2</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>ECM component</t>
+        </is>
+      </c>
+      <c r="D49">
+        <v>21</v>
+      </c>
+      <c r="E49">
+        <v>0.99</v>
+      </c>
+      <c r="F49">
+        <v>0.012</v>
+      </c>
+      <c r="G49">
+        <v>0.84</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>TCGA</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>COL2A1</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>ECM component</t>
+        </is>
+      </c>
+      <c r="D50">
+        <v>1</v>
+      </c>
+      <c r="E50">
+        <v>6.8e-18</v>
+      </c>
+      <c r="F50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>TCGA</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>COL3A1</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>ECM component</t>
+        </is>
+      </c>
+      <c r="D51">
+        <v>21</v>
+      </c>
+      <c r="E51">
+        <v>0.92</v>
+      </c>
+      <c r="F51">
+        <v>0.13</v>
+      </c>
+      <c r="G51">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>TCGA</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>COL4A1</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>ECM component</t>
+        </is>
+      </c>
+      <c r="D52">
+        <v>19</v>
+      </c>
+      <c r="E52">
+        <v>0.89</v>
+      </c>
+      <c r="F52">
+        <v>0</v>
+      </c>
+      <c r="G52">
+        <v>0.9399999999999999</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>TCGA</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>COL4A2</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>ECM component</t>
+        </is>
+      </c>
+      <c r="D53">
+        <v>21</v>
+      </c>
+      <c r="E53">
+        <v>0.97</v>
+      </c>
+      <c r="F53">
+        <v>0</v>
+      </c>
+      <c r="G53">
+        <v>0.86</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>TCGA</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>COL4A3</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>ECM component</t>
+        </is>
+      </c>
+      <c r="D54">
+        <v>10</v>
+      </c>
+      <c r="E54">
+        <v>0.35</v>
+      </c>
+      <c r="F54">
+        <v>0</v>
+      </c>
+      <c r="G54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>TCGA</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>COL4A5</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>ECM component</t>
+        </is>
+      </c>
+      <c r="D55">
+        <v>1</v>
+      </c>
+      <c r="E55">
+        <v>0.0083</v>
+      </c>
+      <c r="F55">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>TCGA</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>COL4A6</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>ECM component</t>
+        </is>
+      </c>
+      <c r="D56">
+        <v>10</v>
+      </c>
+      <c r="E56">
+        <v>0.2</v>
+      </c>
+      <c r="F56">
+        <v>0.76</v>
+      </c>
+      <c r="G56">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>TCGA</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>COL5A1</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>ECM component</t>
+        </is>
+      </c>
+      <c r="D57">
+        <v>21</v>
+      </c>
+      <c r="E57">
+        <v>1</v>
+      </c>
+      <c r="F57">
+        <v>0</v>
+      </c>
+      <c r="G57">
+        <v>0.86</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>TCGA</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>COL5A2</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>ECM component</t>
+        </is>
+      </c>
+      <c r="D58">
+        <v>16</v>
+      </c>
+      <c r="E58">
+        <v>0.74</v>
+      </c>
+      <c r="F58">
+        <v>0.037</v>
+      </c>
+      <c r="G58">
+        <v>0.91</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>TCGA</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>COL6A1</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>ECM component</t>
+        </is>
+      </c>
+      <c r="D59">
+        <v>22</v>
+      </c>
+      <c r="E59">
+        <v>0.91</v>
+      </c>
+      <c r="F59">
+        <v>0.037</v>
+      </c>
+      <c r="G59">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>TCGA</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>COL6A2</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>ECM component</t>
+        </is>
+      </c>
+      <c r="D60">
+        <v>21</v>
+      </c>
+      <c r="E60">
+        <v>0.85</v>
+      </c>
+      <c r="F60">
+        <v>0.11</v>
+      </c>
+      <c r="G60">
+        <v>0.8100000000000001</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>TCGA</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>COL6A3</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>ECM component</t>
+        </is>
+      </c>
+      <c r="D61">
+        <v>23</v>
+      </c>
+      <c r="E61">
+        <v>0.93</v>
+      </c>
+      <c r="F61">
+        <v>0.32</v>
+      </c>
+      <c r="G61">
+        <v>0.6899999999999999</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>TCGA</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>COL7A1</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>ECM component</t>
+        </is>
+      </c>
+      <c r="D62">
+        <v>7</v>
+      </c>
+      <c r="E62">
+        <v>0.1</v>
+      </c>
+      <c r="F62">
+        <v>0.74</v>
+      </c>
+      <c r="G62">
+        <v>0.43</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>TCGA</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>COL9A1</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>ECM component</t>
+        </is>
+      </c>
+      <c r="D63">
+        <v>3</v>
+      </c>
+      <c r="E63">
+        <v>0.0063</v>
+      </c>
+      <c r="F63">
+        <v>0</v>
+      </c>
+      <c r="G63">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>TCGA</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>CTSS</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>ECM processing</t>
+        </is>
+      </c>
+      <c r="D64">
+        <v>6</v>
+      </c>
+      <c r="E64">
+        <v>0.18</v>
+      </c>
+      <c r="F64">
+        <v>0.41</v>
+      </c>
+      <c r="G64">
+        <v>0.67</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>TCGA</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>DST</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>adhesion</t>
+        </is>
+      </c>
+      <c r="D65">
+        <v>5</v>
+      </c>
+      <c r="E65">
+        <v>0.053</v>
+      </c>
+      <c r="F65">
+        <v>0.049</v>
+      </c>
+      <c r="G65">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>TCGA</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>ITGB4</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>adhesion</t>
+        </is>
+      </c>
+      <c r="D66">
+        <v>10</v>
+      </c>
+      <c r="E66">
+        <v>0.11</v>
+      </c>
+      <c r="F66">
+        <v>0.61</v>
+      </c>
+      <c r="G66">
+        <v>0.42</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>TCGA</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>LAMB3</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>ECM component</t>
+        </is>
+      </c>
+      <c r="D67">
+        <v>7</v>
+      </c>
+      <c r="E67">
+        <v>0.026</v>
+      </c>
+      <c r="F67">
+        <v>0</v>
+      </c>
+      <c r="G67">
+        <v>0.57</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>TCGA</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>LAMC2</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>ECM component</t>
+        </is>
+      </c>
+      <c r="D68">
+        <v>1</v>
+      </c>
+      <c r="E68">
+        <v>6.8e-18</v>
+      </c>
+      <c r="F68">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>TCGA</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>LOXL1</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>collagen modification</t>
+        </is>
+      </c>
+      <c r="D69">
+        <v>20</v>
+      </c>
+      <c r="E69">
+        <v>0.89</v>
+      </c>
+      <c r="F69">
+        <v>0.024</v>
+      </c>
+      <c r="G69">
+        <v>0.91</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>TCGA</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>LOXL2</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>collagen modification</t>
+        </is>
+      </c>
+      <c r="D70">
+        <v>19</v>
+      </c>
+      <c r="E70">
+        <v>0.86</v>
+      </c>
+      <c r="F70">
+        <v>0.037</v>
+      </c>
+      <c r="G70">
+        <v>0.9399999999999999</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>TCGA</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>MMP7</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>ECM processing</t>
+        </is>
+      </c>
+      <c r="D71">
+        <v>3</v>
+      </c>
+      <c r="E71">
+        <v>0.0067</v>
+      </c>
+      <c r="F71">
+        <v>0</v>
+      </c>
+      <c r="G71">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>TCGA</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>MMP9</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>ECM processing</t>
+        </is>
+      </c>
+      <c r="D72">
+        <v>1</v>
+      </c>
+      <c r="E72">
+        <v>0.0077</v>
+      </c>
+      <c r="F72">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>TCGA</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>P4HB</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>collagen modification</t>
+        </is>
+      </c>
+      <c r="D73">
+        <v>3</v>
+      </c>
+      <c r="E73">
+        <v>2.7e-17</v>
+      </c>
+      <c r="F73">
+        <v>0.037</v>
+      </c>
+      <c r="G73">
+        <v>0.33</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>TCGA</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>PCOLCE</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>ECM processing</t>
+        </is>
+      </c>
+      <c r="D74">
+        <v>21</v>
+      </c>
+      <c r="E74">
+        <v>0.89</v>
+      </c>
+      <c r="F74">
+        <v>0.024</v>
+      </c>
+      <c r="G74">
+        <v>0.86</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>TCGA</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>PCOLCE2</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>ECM processing</t>
+        </is>
+      </c>
+      <c r="D75">
+        <v>15</v>
+      </c>
+      <c r="E75">
+        <v>0.5600000000000001</v>
+      </c>
+      <c r="F75">
+        <v>0.3</v>
+      </c>
+      <c r="G75">
+        <v>0.84</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>TCGA</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>PLOD1</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>collagen modification</t>
+        </is>
+      </c>
+      <c r="D76">
+        <v>2</v>
+      </c>
+      <c r="E76">
+        <v>1.4e-17</v>
+      </c>
+      <c r="F76">
+        <v>0</v>
+      </c>
+      <c r="G76">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>TCGA</t>
+        </is>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>PPIB</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>collagen modification</t>
+        </is>
+      </c>
+      <c r="D77">
+        <v>3</v>
+      </c>
+      <c r="E77">
+        <v>5.5e-17</v>
+      </c>
+      <c r="F77">
+        <v>0.037</v>
+      </c>
+      <c r="G77">
+        <v>0.33</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>TCGA</t>
+        </is>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>PYCR1</t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>proline metabolism</t>
+        </is>
+      </c>
+      <c r="D78">
+        <v>1</v>
+      </c>
+      <c r="E78">
+        <v>6.8e-18</v>
+      </c>
+      <c r="F78">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>TCGA</t>
+        </is>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>SERPINH1</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>ECM processing</t>
+        </is>
+      </c>
+      <c r="D79">
+        <v>16</v>
+      </c>
+      <c r="E79">
+        <v>0.6</v>
+      </c>
+      <c r="F79">
+        <v>0.037</v>
+      </c>
+      <c r="G79">
+        <v>0.98</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>DKFZ</t>
+        </is>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>ADAMTS2</t>
+        </is>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>ECM processing</t>
+        </is>
+      </c>
+      <c r="D80">
+        <v>17</v>
+      </c>
+      <c r="E80">
+        <v>0.85</v>
+      </c>
+      <c r="F80">
+        <v>0.0046</v>
+      </c>
+      <c r="G80">
+        <v>0.76</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>DKFZ</t>
+        </is>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>ALDH18A1</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>proline metabolism</t>
+        </is>
+      </c>
+      <c r="D81">
+        <v>1</v>
+      </c>
+      <c r="E81">
+        <v>2.5e-05</v>
+      </c>
+      <c r="F81">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>DKFZ</t>
+        </is>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>BMP1</t>
+        </is>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>ECM processing</t>
+        </is>
+      </c>
+      <c r="D82">
+        <v>17</v>
+      </c>
+      <c r="E82">
+        <v>0.72</v>
+      </c>
+      <c r="F82">
+        <v>0.57</v>
+      </c>
+      <c r="G82">
+        <v>0.64</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>DKFZ</t>
+        </is>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>CD151</t>
+        </is>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>adhesion</t>
+        </is>
+      </c>
+      <c r="D83">
+        <v>4</v>
+      </c>
+      <c r="E83">
+        <v>0.0078</v>
+      </c>
+      <c r="F83">
+        <v>0.32</v>
+      </c>
+      <c r="G83">
+        <v>0.17</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>DKFZ</t>
+        </is>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>COL11A1</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>ECM component</t>
+        </is>
+      </c>
+      <c r="D84">
+        <v>6</v>
+      </c>
+      <c r="E84">
+        <v>0.25</v>
+      </c>
+      <c r="F84">
+        <v>0</v>
+      </c>
+      <c r="G84">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>DKFZ</t>
+        </is>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>COL11A2</t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>ECM component</t>
+        </is>
+      </c>
+      <c r="D85">
+        <v>4</v>
+      </c>
+      <c r="E85">
+        <v>0.14</v>
+      </c>
+      <c r="F85">
+        <v>0.037</v>
+      </c>
+      <c r="G85">
+        <v>0.83</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>DKFZ</t>
+        </is>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>COL14A1</t>
+        </is>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>ECM component</t>
+        </is>
+      </c>
+      <c r="D86">
+        <v>6</v>
+      </c>
+      <c r="E86">
+        <v>0.24</v>
+      </c>
+      <c r="F86">
+        <v>0.17</v>
+      </c>
+      <c r="G86">
+        <v>0.67</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>DKFZ</t>
+        </is>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>COL15A1</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>ECM component</t>
+        </is>
+      </c>
+      <c r="D87">
+        <v>14</v>
+      </c>
+      <c r="E87">
+        <v>0.71</v>
+      </c>
+      <c r="F87">
+        <v>0.0046</v>
+      </c>
+      <c r="G87">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>DKFZ</t>
+        </is>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>COL16A1</t>
+        </is>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>ECM component</t>
+        </is>
+      </c>
+      <c r="D88">
+        <v>18</v>
+      </c>
+      <c r="E88">
+        <v>0.82</v>
+      </c>
+      <c r="F88">
+        <v>0.083</v>
+      </c>
+      <c r="G88">
+        <v>0.6899999999999999</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>DKFZ</t>
+        </is>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>COL17A1</t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>ECM component</t>
+        </is>
+      </c>
+      <c r="D89">
+        <v>4</v>
+      </c>
+      <c r="E89">
+        <v>0.028</v>
+      </c>
+      <c r="F89">
+        <v>0.63</v>
+      </c>
+      <c r="G89">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>DKFZ</t>
+        </is>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>COL18A1</t>
+        </is>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>ECM component</t>
+        </is>
+      </c>
+      <c r="D90">
+        <v>15</v>
+      </c>
+      <c r="E90">
+        <v>0.67</v>
+      </c>
+      <c r="F90">
+        <v>0.06</v>
+      </c>
+      <c r="G90">
+        <v>0.73</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>DKFZ</t>
+        </is>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>COL1A1</t>
+        </is>
+      </c>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>ECM component</t>
+        </is>
+      </c>
+      <c r="D91">
+        <v>19</v>
+      </c>
+      <c r="E91">
+        <v>0.95</v>
+      </c>
+      <c r="F91">
+        <v>0.018</v>
+      </c>
+      <c r="G91">
+        <v>0.73</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>DKFZ</t>
+        </is>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>COL1A2</t>
+        </is>
+      </c>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t>ECM component</t>
+        </is>
+      </c>
+      <c r="D92">
+        <v>16</v>
+      </c>
+      <c r="E92">
+        <v>0.8100000000000001</v>
+      </c>
+      <c r="F92">
+        <v>0.074</v>
+      </c>
+      <c r="G92">
+        <v>0.72</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>DKFZ</t>
+        </is>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>COL2A1</t>
+        </is>
+      </c>
+      <c r="C93" t="inlineStr">
+        <is>
+          <t>ECM component</t>
+        </is>
+      </c>
+      <c r="D93">
+        <v>1</v>
+      </c>
+      <c r="E93">
+        <v>6e-18</v>
+      </c>
+      <c r="F93">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>DKFZ</t>
+        </is>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>COL3A1</t>
+        </is>
+      </c>
+      <c r="C94" t="inlineStr">
+        <is>
+          <t>ECM component</t>
+        </is>
+      </c>
+      <c r="D94">
+        <v>13</v>
+      </c>
+      <c r="E94">
+        <v>0.68</v>
+      </c>
+      <c r="F94">
+        <v>0.0092</v>
+      </c>
+      <c r="G94">
+        <v>0.83</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>DKFZ</t>
+        </is>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>COL4A1</t>
+        </is>
+      </c>
+      <c r="C95" t="inlineStr">
+        <is>
+          <t>ECM component</t>
+        </is>
+      </c>
+      <c r="D95">
+        <v>14</v>
+      </c>
+      <c r="E95">
+        <v>0.71</v>
+      </c>
+      <c r="F95">
+        <v>0.06900000000000001</v>
+      </c>
+      <c r="G95">
+        <v>0.79</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>DKFZ</t>
+        </is>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>COL4A2</t>
+        </is>
+      </c>
+      <c r="C96" t="inlineStr">
+        <is>
+          <t>ECM component</t>
+        </is>
+      </c>
+      <c r="D96">
+        <v>18</v>
+      </c>
+      <c r="E96">
+        <v>0.92</v>
+      </c>
+      <c r="F96">
+        <v>0.051</v>
+      </c>
+      <c r="G96">
+        <v>0.74</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>DKFZ</t>
+        </is>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>COL4A3</t>
+        </is>
+      </c>
+      <c r="C97" t="inlineStr">
+        <is>
+          <t>ECM component</t>
+        </is>
+      </c>
+      <c r="D97">
+        <v>1</v>
+      </c>
+      <c r="E97">
+        <v>3.2e-07</v>
+      </c>
+      <c r="F97">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="inlineStr">
+        <is>
+          <t>DKFZ</t>
+        </is>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>COL4A5</t>
+        </is>
+      </c>
+      <c r="C98" t="inlineStr">
+        <is>
+          <t>ECM component</t>
+        </is>
+      </c>
+      <c r="D98">
+        <v>2</v>
+      </c>
+      <c r="E98">
+        <v>0.0001</v>
+      </c>
+      <c r="F98">
+        <v>0.33</v>
+      </c>
+      <c r="G98">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="inlineStr">
+        <is>
+          <t>DKFZ</t>
+        </is>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>COL4A6</t>
+        </is>
+      </c>
+      <c r="C99" t="inlineStr">
+        <is>
+          <t>ECM component</t>
+        </is>
+      </c>
+      <c r="D99">
+        <v>2</v>
+      </c>
+      <c r="E99">
+        <v>0.0017</v>
+      </c>
+      <c r="F99">
+        <v>0.48</v>
+      </c>
+      <c r="G99">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="inlineStr">
+        <is>
+          <t>DKFZ</t>
+        </is>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>COL5A1</t>
+        </is>
+      </c>
+      <c r="C100" t="inlineStr">
+        <is>
+          <t>ECM component</t>
+        </is>
+      </c>
+      <c r="D100">
+        <v>19</v>
+      </c>
+      <c r="E100">
+        <v>1</v>
+      </c>
+      <c r="F100">
+        <v>0.055</v>
+      </c>
+      <c r="G100">
+        <v>0.72</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="inlineStr">
+        <is>
+          <t>DKFZ</t>
+        </is>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>COL5A2</t>
+        </is>
+      </c>
+      <c r="C101" t="inlineStr">
+        <is>
+          <t>ECM component</t>
+        </is>
+      </c>
+      <c r="D101">
+        <v>11</v>
+      </c>
+      <c r="E101">
+        <v>0.59</v>
+      </c>
+      <c r="F101">
+        <v>0.0046</v>
+      </c>
+      <c r="G101">
+        <v>0.91</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="inlineStr">
+        <is>
+          <t>DKFZ</t>
+        </is>
+      </c>
+      <c r="B102" t="inlineStr">
+        <is>
+          <t>COL6A1</t>
+        </is>
+      </c>
+      <c r="C102" t="inlineStr">
+        <is>
+          <t>ECM component</t>
+        </is>
+      </c>
+      <c r="D102">
+        <v>19</v>
+      </c>
+      <c r="E102">
+        <v>0.85</v>
+      </c>
+      <c r="F102">
+        <v>0.47</v>
+      </c>
+      <c r="G102">
+        <v>0.66</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>DKFZ</t>
+        </is>
+      </c>
+      <c r="B103" t="inlineStr">
+        <is>
+          <t>COL6A2</t>
+        </is>
+      </c>
+      <c r="C103" t="inlineStr">
+        <is>
+          <t>ECM component</t>
+        </is>
+      </c>
+      <c r="D103">
+        <v>14</v>
+      </c>
+      <c r="E103">
+        <v>0.67</v>
+      </c>
+      <c r="F103">
+        <v>0.097</v>
+      </c>
+      <c r="G103">
+        <v>0.78</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="inlineStr">
+        <is>
+          <t>DKFZ</t>
+        </is>
+      </c>
+      <c r="B104" t="inlineStr">
+        <is>
+          <t>COL6A3</t>
+        </is>
+      </c>
+      <c r="C104" t="inlineStr">
+        <is>
+          <t>ECM component</t>
+        </is>
+      </c>
+      <c r="D104">
+        <v>17</v>
+      </c>
+      <c r="E104">
+        <v>0.8100000000000001</v>
+      </c>
+      <c r="F104">
+        <v>0.06900000000000001</v>
+      </c>
+      <c r="G104">
+        <v>0.73</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="inlineStr">
+        <is>
+          <t>DKFZ</t>
+        </is>
+      </c>
+      <c r="B105" t="inlineStr">
+        <is>
+          <t>COL7A1</t>
+        </is>
+      </c>
+      <c r="C105" t="inlineStr">
+        <is>
+          <t>ECM component</t>
+        </is>
+      </c>
+      <c r="D105">
+        <v>8</v>
+      </c>
+      <c r="E105">
+        <v>0.2</v>
+      </c>
+      <c r="F105">
+        <v>0.76</v>
+      </c>
+      <c r="G105">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="inlineStr">
+        <is>
+          <t>DKFZ</t>
+        </is>
+      </c>
+      <c r="B106" t="inlineStr">
+        <is>
+          <t>COL9A3</t>
+        </is>
+      </c>
+      <c r="C106" t="inlineStr">
+        <is>
+          <t>ECM component</t>
+        </is>
+      </c>
+      <c r="D106">
+        <v>1</v>
+      </c>
+      <c r="E106">
+        <v>6e-18</v>
+      </c>
+      <c r="F106">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="inlineStr">
+        <is>
+          <t>DKFZ</t>
+        </is>
+      </c>
+      <c r="B107" t="inlineStr">
+        <is>
+          <t>CTSS</t>
+        </is>
+      </c>
+      <c r="C107" t="inlineStr">
+        <is>
+          <t>ECM processing</t>
+        </is>
+      </c>
+      <c r="D107">
+        <v>1</v>
+      </c>
+      <c r="E107">
+        <v>1.8e-17</v>
+      </c>
+      <c r="F107">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="inlineStr">
+        <is>
+          <t>DKFZ</t>
+        </is>
+      </c>
+      <c r="B108" t="inlineStr">
+        <is>
+          <t>DST</t>
+        </is>
+      </c>
+      <c r="C108" t="inlineStr">
+        <is>
+          <t>adhesion</t>
+        </is>
+      </c>
+      <c r="D108">
+        <v>2</v>
+      </c>
+      <c r="E108">
+        <v>5.1e-06</v>
+      </c>
+      <c r="F108">
+        <v>0.17</v>
+      </c>
+      <c r="G108">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="inlineStr">
+        <is>
+          <t>DKFZ</t>
+        </is>
+      </c>
+      <c r="B109" t="inlineStr">
+        <is>
+          <t>ITGB4</t>
+        </is>
+      </c>
+      <c r="C109" t="inlineStr">
+        <is>
+          <t>adhesion</t>
+        </is>
+      </c>
+      <c r="D109">
+        <v>9</v>
+      </c>
+      <c r="E109">
+        <v>0.27</v>
+      </c>
+      <c r="F109">
+        <v>0.12</v>
+      </c>
+      <c r="G109">
+        <v>0.58</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="inlineStr">
+        <is>
+          <t>DKFZ</t>
+        </is>
+      </c>
+      <c r="B110" t="inlineStr">
+        <is>
+          <t>LAMB3</t>
+        </is>
+      </c>
+      <c r="C110" t="inlineStr">
+        <is>
+          <t>ECM component</t>
+        </is>
+      </c>
+      <c r="D110">
+        <v>3</v>
+      </c>
+      <c r="E110">
+        <v>0.034</v>
+      </c>
+      <c r="F110">
+        <v>0</v>
+      </c>
+      <c r="G110">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="inlineStr">
+        <is>
+          <t>DKFZ</t>
+        </is>
+      </c>
+      <c r="B111" t="inlineStr">
+        <is>
+          <t>LOXL1</t>
+        </is>
+      </c>
+      <c r="C111" t="inlineStr">
+        <is>
+          <t>collagen modification</t>
+        </is>
+      </c>
+      <c r="D111">
+        <v>19</v>
+      </c>
+      <c r="E111">
+        <v>0.92</v>
+      </c>
+      <c r="F111">
+        <v>0.032</v>
+      </c>
+      <c r="G111">
+        <v>0.71</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="inlineStr">
+        <is>
+          <t>DKFZ</t>
+        </is>
+      </c>
+      <c r="B112" t="inlineStr">
+        <is>
+          <t>LOXL2</t>
+        </is>
+      </c>
+      <c r="C112" t="inlineStr">
+        <is>
+          <t>collagen modification</t>
+        </is>
+      </c>
+      <c r="D112">
+        <v>15</v>
+      </c>
+      <c r="E112">
+        <v>0.7</v>
+      </c>
+      <c r="F112">
+        <v>0.051</v>
+      </c>
+      <c r="G112">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="inlineStr">
+        <is>
+          <t>DKFZ</t>
+        </is>
+      </c>
+      <c r="B113" t="inlineStr">
+        <is>
+          <t>MMP9</t>
+        </is>
+      </c>
+      <c r="C113" t="inlineStr">
+        <is>
+          <t>ECM processing</t>
+        </is>
+      </c>
+      <c r="D113">
+        <v>1</v>
+      </c>
+      <c r="E113">
+        <v>1.8e-17</v>
+      </c>
+      <c r="F113">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="inlineStr">
+        <is>
+          <t>DKFZ</t>
+        </is>
+      </c>
+      <c r="B114" t="inlineStr">
+        <is>
+          <t>P4HA1</t>
+        </is>
+      </c>
+      <c r="C114" t="inlineStr">
+        <is>
+          <t>collagen modification</t>
+        </is>
+      </c>
+      <c r="D114">
+        <v>1</v>
+      </c>
+      <c r="E114">
+        <v>1.8e-17</v>
+      </c>
+      <c r="F114">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="inlineStr">
+        <is>
+          <t>DKFZ</t>
+        </is>
+      </c>
+      <c r="B115" t="inlineStr">
+        <is>
+          <t>P4HB</t>
+        </is>
+      </c>
+      <c r="C115" t="inlineStr">
+        <is>
+          <t>collagen modification</t>
+        </is>
+      </c>
+      <c r="D115">
+        <v>3</v>
+      </c>
+      <c r="E115">
+        <v>0.00073</v>
+      </c>
+      <c r="F115">
+        <v>0.0092</v>
+      </c>
+      <c r="G115">
+        <v>0.33</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="inlineStr">
+        <is>
+          <t>DKFZ</t>
+        </is>
+      </c>
+      <c r="B116" t="inlineStr">
+        <is>
+          <t>PCOLCE</t>
+        </is>
+      </c>
+      <c r="C116" t="inlineStr">
+        <is>
+          <t>ECM processing</t>
+        </is>
+      </c>
+      <c r="D116">
+        <v>12</v>
+      </c>
+      <c r="E116">
+        <v>0.58</v>
+      </c>
+      <c r="F116">
+        <v>0.06</v>
+      </c>
+      <c r="G116">
+        <v>0.86</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="inlineStr">
+        <is>
+          <t>DKFZ</t>
+        </is>
+      </c>
+      <c r="B117" t="inlineStr">
+        <is>
+          <t>PCOLCE2</t>
+        </is>
+      </c>
+      <c r="C117" t="inlineStr">
+        <is>
+          <t>ECM processing</t>
+        </is>
+      </c>
+      <c r="D117">
+        <v>1</v>
+      </c>
+      <c r="E117">
+        <v>0.015</v>
+      </c>
+      <c r="F117">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="inlineStr">
+        <is>
+          <t>DKFZ</t>
+        </is>
+      </c>
+      <c r="B118" t="inlineStr">
+        <is>
+          <t>PEPD</t>
+        </is>
+      </c>
+      <c r="C118" t="inlineStr">
+        <is>
+          <t>proline metabolism</t>
+        </is>
+      </c>
+      <c r="D118">
+        <v>1</v>
+      </c>
+      <c r="E118">
+        <v>0.0004</v>
+      </c>
+      <c r="F118">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="inlineStr">
+        <is>
+          <t>DKFZ</t>
+        </is>
+      </c>
+      <c r="B119" t="inlineStr">
+        <is>
+          <t>PLOD1</t>
+        </is>
+      </c>
+      <c r="C119" t="inlineStr">
+        <is>
+          <t>collagen modification</t>
+        </is>
+      </c>
+      <c r="D119">
+        <v>4</v>
+      </c>
+      <c r="E119">
+        <v>0.009599999999999999</v>
+      </c>
+      <c r="F119">
+        <v>0.46</v>
+      </c>
+      <c r="G119">
+        <v>0.33</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="inlineStr">
+        <is>
+          <t>DKFZ</t>
+        </is>
+      </c>
+      <c r="B120" t="inlineStr">
+        <is>
+          <t>PLOD2</t>
+        </is>
+      </c>
+      <c r="C120" t="inlineStr">
+        <is>
+          <t>collagen modification</t>
+        </is>
+      </c>
+      <c r="D120">
+        <v>1</v>
+      </c>
+      <c r="E120">
+        <v>1.8e-17</v>
+      </c>
+      <c r="F120">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="inlineStr">
+        <is>
+          <t>DKFZ</t>
+        </is>
+      </c>
+      <c r="B121" t="inlineStr">
+        <is>
+          <t>PLOD3</t>
+        </is>
+      </c>
+      <c r="C121" t="inlineStr">
+        <is>
+          <t>collagen modification</t>
+        </is>
+      </c>
+      <c r="D121">
+        <v>6</v>
+      </c>
+      <c r="E121">
+        <v>0.15</v>
+      </c>
+      <c r="F121">
+        <v>1</v>
+      </c>
+      <c r="G121">
+        <v>0.47</v>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="inlineStr">
+        <is>
+          <t>DKFZ</t>
+        </is>
+      </c>
+      <c r="B122" t="inlineStr">
+        <is>
+          <t>PPIB</t>
+        </is>
+      </c>
+      <c r="C122" t="inlineStr">
+        <is>
+          <t>collagen modification</t>
+        </is>
+      </c>
+      <c r="D122">
+        <v>3</v>
+      </c>
+      <c r="E122">
+        <v>0.00052</v>
+      </c>
+      <c r="F122">
+        <v>0.17</v>
+      </c>
+      <c r="G122">
+        <v>0.33</v>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="inlineStr">
+        <is>
+          <t>DKFZ</t>
+        </is>
+      </c>
+      <c r="B123" t="inlineStr">
+        <is>
+          <t>PYCR1</t>
+        </is>
+      </c>
+      <c r="C123" t="inlineStr">
+        <is>
+          <t>proline metabolism</t>
+        </is>
+      </c>
+      <c r="D123">
+        <v>2</v>
+      </c>
+      <c r="E123">
+        <v>0.00045</v>
+      </c>
+      <c r="F123">
+        <v>0.0092</v>
+      </c>
+      <c r="G123">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="inlineStr">
+        <is>
+          <t>DKFZ</t>
+        </is>
+      </c>
+      <c r="B124" t="inlineStr">
+        <is>
+          <t>SERPINH1</t>
+        </is>
+      </c>
+      <c r="C124" t="inlineStr">
+        <is>
+          <t>ECM processing</t>
+        </is>
+      </c>
+      <c r="D124">
+        <v>15</v>
+      </c>
+      <c r="E124">
+        <v>0.65</v>
+      </c>
+      <c r="F124">
+        <v>0.41</v>
+      </c>
+      <c r="G124">
+        <v>0.76</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
ROC analyses for BCR
Analysis of prediction of VCR at one, two. three, and five year follow-up by ROC. Inference for the GBM models
</commit_message>
<xml_diff>
--- a/paper/supplementary_tables.xlsx
+++ b/paper/supplementary_tables.xlsx
@@ -18,6 +18,7 @@
     <sheet name="Supplementary Table S8" sheetId="9" r:id="rId9"/>
     <sheet name="Supplementary Table S9" sheetId="10" r:id="rId10"/>
     <sheet name="Supplementary Table S10" sheetId="11" r:id="rId11"/>
+    <sheet name="Supplementary Table S11" sheetId="12" r:id="rId12"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -361,7 +362,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -483,7 +484,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Selection of the optimal parameters of machine learning models of overall survival (OS) in the training subset of the GSE16560 cohort. The models used log2 expression of the collagen-related genes as explanatory variables.</t>
+          <t>Prediction of biochemical relapse (BCR) at one, two, three, and five year after diagnosis by gradient boosted models employing clinical predictors and expression of the collagen-related transcrips as explanatory factors.</t>
         </is>
       </c>
     </row>
@@ -494,6 +495,18 @@
         </is>
       </c>
       <c r="B11" t="inlineStr">
+        <is>
+          <t>Selection of the optimal parameters of machine learning models of overall survival (OS) in the training subset of the GSE16560 cohort. The models used log2 expression of the collagen-related genes as explanatory variables.</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Supplementary Table S11</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
         <is>
           <t>Performance of machine learning models at prediction of overall survival (OS) in the training and test subsets of the GSE16560 cohort. The models used log2 expression of the collagen-related genes as explanatory factors.</t>
         </is>
@@ -505,6 +518,915 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:F37"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" s="1" customFormat="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Time after diagnosis, months</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Cohort</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Model</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Total patients, N</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Fraction of BCR</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>ROC AUC</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2">
+        <v>12</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>pooled GEO</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>GBM, expression</t>
+        </is>
+      </c>
+      <c r="D2">
+        <v>485</v>
+      </c>
+      <c r="E2">
+        <v>0.12</v>
+      </c>
+      <c r="F2">
+        <v>0.91</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3">
+        <v>12</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>pooled GEO</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>GBM, clinic</t>
+        </is>
+      </c>
+      <c r="D3">
+        <v>465</v>
+      </c>
+      <c r="E3">
+        <v>0.13</v>
+      </c>
+      <c r="F3">
+        <v>0.78</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4">
+        <v>12</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>pooled GEO</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>GBM, clinic + expression</t>
+        </is>
+      </c>
+      <c r="D4">
+        <v>465</v>
+      </c>
+      <c r="E4">
+        <v>0.13</v>
+      </c>
+      <c r="F4">
+        <v>0.89</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5">
+        <v>12</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>TCGA</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>GBM, expression</t>
+        </is>
+      </c>
+      <c r="D5">
+        <v>493</v>
+      </c>
+      <c r="E5">
+        <v>0.062</v>
+      </c>
+      <c r="F5">
+        <v>0.67</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6">
+        <v>12</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>TCGA</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>GBM, clinic</t>
+        </is>
+      </c>
+      <c r="D6">
+        <v>476</v>
+      </c>
+      <c r="E6">
+        <v>0.06</v>
+      </c>
+      <c r="F6">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7">
+        <v>12</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>TCGA</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>GBM, clinic + expression</t>
+        </is>
+      </c>
+      <c r="D7">
+        <v>476</v>
+      </c>
+      <c r="E7">
+        <v>0.06</v>
+      </c>
+      <c r="F7">
+        <v>0.66</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8">
+        <v>12</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>DKFZ</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>GBM, expression</t>
+        </is>
+      </c>
+      <c r="D8">
+        <v>105</v>
+      </c>
+      <c r="E8">
+        <v>0.17</v>
+      </c>
+      <c r="F8">
+        <v>0.88</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9">
+        <v>12</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>DKFZ</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>GBM, clinic</t>
+        </is>
+      </c>
+      <c r="D9">
+        <v>98</v>
+      </c>
+      <c r="E9">
+        <v>0.13</v>
+      </c>
+      <c r="F9">
+        <v>0.71</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10">
+        <v>12</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>DKFZ</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>GBM, clinic + expression</t>
+        </is>
+      </c>
+      <c r="D10">
+        <v>98</v>
+      </c>
+      <c r="E10">
+        <v>0.13</v>
+      </c>
+      <c r="F10">
+        <v>0.8100000000000001</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11">
+        <v>24</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>pooled GEO</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>GBM, expression</t>
+        </is>
+      </c>
+      <c r="D11">
+        <v>485</v>
+      </c>
+      <c r="E11">
+        <v>0.21</v>
+      </c>
+      <c r="F11">
+        <v>0.92</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12">
+        <v>24</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>pooled GEO</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>GBM, clinic</t>
+        </is>
+      </c>
+      <c r="D12">
+        <v>465</v>
+      </c>
+      <c r="E12">
+        <v>0.21</v>
+      </c>
+      <c r="F12">
+        <v>0.77</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13">
+        <v>24</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>pooled GEO</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>GBM, clinic + expression</t>
+        </is>
+      </c>
+      <c r="D13">
+        <v>465</v>
+      </c>
+      <c r="E13">
+        <v>0.21</v>
+      </c>
+      <c r="F13">
+        <v>0.91</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14">
+        <v>24</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>TCGA</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>GBM, expression</t>
+        </is>
+      </c>
+      <c r="D14">
+        <v>493</v>
+      </c>
+      <c r="E14">
+        <v>0.13</v>
+      </c>
+      <c r="F14">
+        <v>0.64</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15">
+        <v>24</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>TCGA</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>GBM, clinic</t>
+        </is>
+      </c>
+      <c r="D15">
+        <v>476</v>
+      </c>
+      <c r="E15">
+        <v>0.13</v>
+      </c>
+      <c r="F15">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16">
+        <v>24</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>TCGA</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>GBM, clinic + expression</t>
+        </is>
+      </c>
+      <c r="D16">
+        <v>476</v>
+      </c>
+      <c r="E16">
+        <v>0.13</v>
+      </c>
+      <c r="F16">
+        <v>0.66</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17">
+        <v>24</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>DKFZ</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>GBM, expression</t>
+        </is>
+      </c>
+      <c r="D17">
+        <v>105</v>
+      </c>
+      <c r="E17">
+        <v>0.22</v>
+      </c>
+      <c r="F17">
+        <v>0.8100000000000001</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18">
+        <v>24</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>DKFZ</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>GBM, clinic</t>
+        </is>
+      </c>
+      <c r="D18">
+        <v>98</v>
+      </c>
+      <c r="E18">
+        <v>0.17</v>
+      </c>
+      <c r="F18">
+        <v>0.65</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19">
+        <v>24</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>DKFZ</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>GBM, clinic + expression</t>
+        </is>
+      </c>
+      <c r="D19">
+        <v>98</v>
+      </c>
+      <c r="E19">
+        <v>0.17</v>
+      </c>
+      <c r="F19">
+        <v>0.79</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20">
+        <v>36</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>pooled GEO</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>GBM, expression</t>
+        </is>
+      </c>
+      <c r="D20">
+        <v>485</v>
+      </c>
+      <c r="E20">
+        <v>0.27</v>
+      </c>
+      <c r="F20">
+        <v>0.92</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21">
+        <v>36</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>pooled GEO</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>GBM, clinic</t>
+        </is>
+      </c>
+      <c r="D21">
+        <v>465</v>
+      </c>
+      <c r="E21">
+        <v>0.27</v>
+      </c>
+      <c r="F21">
+        <v>0.76</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22">
+        <v>36</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>pooled GEO</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>GBM, clinic + expression</t>
+        </is>
+      </c>
+      <c r="D22">
+        <v>465</v>
+      </c>
+      <c r="E22">
+        <v>0.27</v>
+      </c>
+      <c r="F22">
+        <v>0.92</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23">
+        <v>36</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>TCGA</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>GBM, expression</t>
+        </is>
+      </c>
+      <c r="D23">
+        <v>493</v>
+      </c>
+      <c r="E23">
+        <v>0.19</v>
+      </c>
+      <c r="F23">
+        <v>0.66</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24">
+        <v>36</v>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>TCGA</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>GBM, clinic</t>
+        </is>
+      </c>
+      <c r="D24">
+        <v>476</v>
+      </c>
+      <c r="E24">
+        <v>0.19</v>
+      </c>
+      <c r="F24">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25">
+        <v>36</v>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>TCGA</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>GBM, clinic + expression</t>
+        </is>
+      </c>
+      <c r="D25">
+        <v>476</v>
+      </c>
+      <c r="E25">
+        <v>0.19</v>
+      </c>
+      <c r="F25">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26">
+        <v>36</v>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>DKFZ</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>GBM, expression</t>
+        </is>
+      </c>
+      <c r="D26">
+        <v>105</v>
+      </c>
+      <c r="E26">
+        <v>0.23</v>
+      </c>
+      <c r="F26">
+        <v>0.78</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27">
+        <v>36</v>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>DKFZ</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>GBM, clinic</t>
+        </is>
+      </c>
+      <c r="D27">
+        <v>98</v>
+      </c>
+      <c r="E27">
+        <v>0.18</v>
+      </c>
+      <c r="F27">
+        <v>0.67</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28">
+        <v>36</v>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>DKFZ</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>GBM, clinic + expression</t>
+        </is>
+      </c>
+      <c r="D28">
+        <v>98</v>
+      </c>
+      <c r="E28">
+        <v>0.18</v>
+      </c>
+      <c r="F28">
+        <v>0.77</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29">
+        <v>60</v>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>pooled GEO</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>GBM, expression</t>
+        </is>
+      </c>
+      <c r="D29">
+        <v>485</v>
+      </c>
+      <c r="E29">
+        <v>0.36</v>
+      </c>
+      <c r="F29">
+        <v>0.92</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30">
+        <v>60</v>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>pooled GEO</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>GBM, clinic</t>
+        </is>
+      </c>
+      <c r="D30">
+        <v>465</v>
+      </c>
+      <c r="E30">
+        <v>0.36</v>
+      </c>
+      <c r="F30">
+        <v>0.78</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31">
+        <v>60</v>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>pooled GEO</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>GBM, clinic + expression</t>
+        </is>
+      </c>
+      <c r="D31">
+        <v>465</v>
+      </c>
+      <c r="E31">
+        <v>0.36</v>
+      </c>
+      <c r="F31">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32">
+        <v>60</v>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>TCGA</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>GBM, expression</t>
+        </is>
+      </c>
+      <c r="D32">
+        <v>493</v>
+      </c>
+      <c r="E32">
+        <v>0.3</v>
+      </c>
+      <c r="F32">
+        <v>0.62</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33">
+        <v>60</v>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>TCGA</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>GBM, clinic</t>
+        </is>
+      </c>
+      <c r="D33">
+        <v>476</v>
+      </c>
+      <c r="E33">
+        <v>0.3</v>
+      </c>
+      <c r="F33">
+        <v>0.74</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34">
+        <v>60</v>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>TCGA</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>GBM, clinic + expression</t>
+        </is>
+      </c>
+      <c r="D34">
+        <v>476</v>
+      </c>
+      <c r="E34">
+        <v>0.3</v>
+      </c>
+      <c r="F34">
+        <v>0.68</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35">
+        <v>60</v>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>DKFZ</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>GBM, expression</t>
+        </is>
+      </c>
+      <c r="D35">
+        <v>105</v>
+      </c>
+      <c r="E35">
+        <v>0.25</v>
+      </c>
+      <c r="F35">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36">
+        <v>60</v>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>DKFZ</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>GBM, clinic</t>
+        </is>
+      </c>
+      <c r="D36">
+        <v>98</v>
+      </c>
+      <c r="E36">
+        <v>0.2</v>
+      </c>
+      <c r="F36">
+        <v>0.68</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37">
+        <v>60</v>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>DKFZ</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>GBM, clinic + expression</t>
+        </is>
+      </c>
+      <c r="D37">
+        <v>98</v>
+      </c>
+      <c r="E37">
+        <v>0.2</v>
+      </c>
+      <c r="F37">
+        <v>0.79</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C7"/>
   <sheetViews>
@@ -650,7 +1572,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D13"/>
   <sheetViews>

</xml_diff>